<commit_message>
Add new Excel file with product codes for third delivery
</commit_message>
<xml_diff>
--- a/data/bsale_primera_entrega.xlsx
+++ b/data/bsale_primera_entrega.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F128900-A4F4-A24D-910A-53F27D34E520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36389ED-736C-CA43-A0C9-1C2827F61B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38560" yWindow="980" windowWidth="38400" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -815,6 +815,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -849,20 +863,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -877,7 +877,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61379E7E-0C23-C04D-BBB0-FB5649CA84CF}" name="Tabla1" displayName="Tabla1" ref="A1:Q96" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61379E7E-0C23-C04D-BBB0-FB5649CA84CF}" name="Tabla1" displayName="Tabla1" ref="A1:Q96" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:Q96" xr:uid="{61379E7E-0C23-C04D-BBB0-FB5649CA84CF}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{EB534F00-11DE-144E-92F5-EF2C2621C0BC}" name="Clasificación"/>
@@ -1190,7 +1190,7 @@
   <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1203,7 +1203,7 @@
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="13" width="16.5" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
     <col min="15" max="15" width="18.83203125" customWidth="1"/>

</xml_diff>